<commit_message>
added clean to pom- initiate with -Pci clean
</commit_message>
<xml_diff>
--- a/c:\timerResults.xlsx
+++ b/c:\timerResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="317">
   <si>
     <t>Test Parameters</t>
   </si>
@@ -942,6 +942,27 @@
   </si>
   <si>
     <t>PRIVATE:Raj_SalesForceCaseScript_16-08-04_13_22_43_99183.xml</t>
+  </si>
+  <si>
+    <t>https://salesforce.perfectomobile.com/services/reports/PRIVATE:Raj_SalesForceCaseScript_16-08-04_13_37_43_99227.xml?operation=download&amp;format=html&amp;user=rajp@perfectomobile.com&amp;password=</t>
+  </si>
+  <si>
+    <t>04/08/2016 09:37:43</t>
+  </si>
+  <si>
+    <t>8759</t>
+  </si>
+  <si>
+    <t>6770</t>
+  </si>
+  <si>
+    <t>3980</t>
+  </si>
+  <si>
+    <t>https://demo.vod-download-01.perfectomobile.com/demo/647672315467564c494d713734357762553872464b7a326b6638337439776b4c4c6c5a55703352456c31453d/877772dae0f270833cc141538dfe10f7f1b12bd16b44b08802322d2518240e5e.flv</t>
+  </si>
+  <si>
+    <t>PRIVATE:Raj_SalesForceCaseScript_16-08-04_13_37_43_99227.xml</t>
   </si>
 </sst>
 </file>
@@ -2006,6 +2027,32 @@
         <v>309</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>310</v>
+      </c>
+      <c r="B40" t="s">
+        <v>311</v>
+      </c>
+      <c r="C40" t="s">
+        <v>116</v>
+      </c>
+      <c r="D40" t="s">
+        <v>312</v>
+      </c>
+      <c r="E40" t="s">
+        <v>313</v>
+      </c>
+      <c r="F40" t="s">
+        <v>314</v>
+      </c>
+      <c r="G40" t="s">
+        <v>315</v>
+      </c>
+      <c r="H40" t="s">
+        <v>316</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>